<commit_message>
Classes, Enums & Primary Key creating
Errors with linked elements still occuring, wihich will not be eliminated until the foreign key code is in place.
</commit_message>
<xml_diff>
--- a/Documentation/SQL Server Data Type Mapping.xlsx
+++ b/Documentation/SQL Server Data Type Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Repos\LightosTomJ\XmlSchemaSQLClassGenerator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44407900-49F1-4930-976A-AD915197B486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E702B6-320E-40BC-82EC-87CA5802D72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{2EBCF0CA-1BBD-4416-BD84-C9160D9783C5}"/>
+    <workbookView xWindow="25500" yWindow="-14250" windowWidth="25820" windowHeight="14020" xr2:uid="{2EBCF0CA-1BBD-4416-BD84-C9160D9783C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL Server" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
   <si>
     <t>Description</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>System.Single</t>
+  </si>
+  <si>
+    <t>SEARCHABLE</t>
   </si>
 </sst>
 </file>
@@ -378,12 +381,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -396,6 +396,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -417,15 +423,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46AC3823-1A3F-4761-AE0B-C8B16F850C42}" name="Table1" displayName="Table1" ref="A1:G36" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:G36" xr:uid="{A484FC31-AADA-4E4C-9A35-3CFA276EC4A6}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46AC3823-1A3F-4761-AE0B-C8B16F850C42}" name="Table1" displayName="Table1" ref="A1:H36" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H36" xr:uid="{A484FC31-AADA-4E4C-9A35-3CFA276EC4A6}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8071A964-D957-4E5D-9D94-CDD2BCFC720D}" name="Category" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{AD035300-63E1-4FF5-83F2-CE4ABEDB3409}" name="VS.Net Type" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{CB955490-B800-46F0-BD9D-08047E39A4CE}" name="SQL Data type" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E25ED441-D357-49AB-B233-09454A354217}" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{13525C3A-CA9B-42DB-B7AB-FF6D3F2D643D}" name="Storage" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{19B6C793-CB81-4243-89C2-337052737FCF}" name="Max size" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{AD035300-63E1-4FF5-83F2-CE4ABEDB3409}" name="VS.Net Type" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CB955490-B800-46F0-BD9D-08047E39A4CE}" name="SQL Data type" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{606148DF-C255-4122-95F2-69D75DEFD3BE}" name="SEARCHABLE" dataDxfId="0">
+      <calculatedColumnFormula>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E25ED441-D357-49AB-B233-09454A354217}" name="Description" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{13525C3A-CA9B-42DB-B7AB-FF6D3F2D643D}" name="Storage" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{19B6C793-CB81-4243-89C2-337052737FCF}" name="Max size" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{57F8925F-7F1A-4B66-9800-60148EC9CCD9}" name="Enum" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</calculatedColumnFormula>
     </tableColumn>
@@ -731,23 +740,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0622978-7C17-40AE-B19F-5EC9DE1E88C1}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" customWidth="1"/>
-    <col min="4" max="4" width="123.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="3" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="123.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -758,19 +767,22 @@
         <v>94</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -778,21 +790,25 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"CHAR",</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="H2" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>CHAR_N_ = 1,</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -800,21 +816,25 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"VARCHAR",</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="H3" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>VARCHAR_N_ = 2,</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -822,21 +842,25 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"VARCHAR",</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="H4" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>VARCHAR_MAX_ = 3,</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -844,21 +868,25 @@
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"TEXT",</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="H5" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>TEXT = 4,</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -866,21 +894,25 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"NCHAR",</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="H6" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>NCHAR = 5,</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -888,21 +920,25 @@
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"NVARCHAR",</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="H7" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>NVARCHAR = 6,</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -910,21 +946,25 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"NVARCHAR",</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="H8" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>NVARCHAR_MAX_ = 7,</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -932,21 +972,25 @@
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"NTEXT",</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="H9" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>NTEXT = 8,</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -954,21 +998,25 @@
       <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"BINARY",</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="1" t="str">
+      <c r="H10" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>BINARY_N_ = 9,</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -976,21 +1024,25 @@
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"VARBINARY",</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="H11" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>VARBINARY = 10,</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -998,21 +1050,25 @@
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"VARBINARY",</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="1" t="str">
+      <c r="H12" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>VARBINARY_MAX_ = 11,</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1020,21 +1076,25 @@
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"IMAGE",</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="1" t="str">
+      <c r="H13" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>IMAGE = 12,</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1042,17 +1102,21 @@
       <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"BIT",</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="str">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>BIT = 13,</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,19 +1124,23 @@
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"TINYINT",</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="str">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>TINYINT = 14,</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1080,19 +1148,23 @@
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"SMALLINT",</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="str">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>SMALLINT = 15,</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1102,19 +1174,23 @@
       <c r="C17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"INT",</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="str">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>INT = 16,</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1124,19 +1200,23 @@
       <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"BIGINT",</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="str">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>BIGINT = 17,</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1144,19 +1224,23 @@
       <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"DECIMAL",</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="str">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>DECIMAL_P-S_ = 18,</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1164,19 +1248,23 @@
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"NUMERIC",</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="str">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>NUMERIC_P-S_ = 19,</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1184,19 +1272,23 @@
       <c r="C21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"SMALLMONEY",</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="str">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>SMALLMONEY = 20,</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1204,19 +1296,23 @@
       <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"MONEY",</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="str">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>MONEY = 21,</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1224,19 +1320,23 @@
       <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"FLOAT",</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="str">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>FLOAT_N_ = 22,</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1244,19 +1344,23 @@
       <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"REAL",</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="str">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>REAL = 23,</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
@@ -1264,19 +1368,23 @@
       <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"DATETIME",</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1" t="str">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>DATETIME = 24,</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -1284,19 +1392,23 @@
       <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"DATETIME2",</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="str">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>DATETIME2 = 25,</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
@@ -1304,19 +1416,23 @@
       <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"SMALLDATETIME",</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="str">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>SMALLDATETIME = 26,</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -1324,19 +1440,23 @@
       <c r="C28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"DATE",</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="str">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>DATE = 27,</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
@@ -1344,19 +1464,23 @@
       <c r="C29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"TIME",</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="str">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>TIME = 28,</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -1364,19 +1488,23 @@
       <c r="C30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"DATETIMEOFFSET",</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="str">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>DATETIMEOFFSET = 29,</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
@@ -1384,19 +1512,23 @@
       <c r="C31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"TIMESTAMP",</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="str">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>TIMESTAMP = 30,</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
@@ -1404,17 +1536,21 @@
       <c r="C32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"SQL_VARIANT",</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1" t="str">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>SQL_VARIANT = 31,</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
@@ -1422,17 +1558,21 @@
       <c r="C33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"UNIQUEIDENTIFIER",</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1" t="str">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>UNIQUEIDENTIFIER = 32,</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
@@ -1440,17 +1580,21 @@
       <c r="C34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"XML",</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1" t="str">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>XML = 33,</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -1458,17 +1602,21 @@
       <c r="C35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"CURSOR",</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1" t="str">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>CURSOR = 34,</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
@@ -1476,12 +1624,16 @@
       <c r="C36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="str">
+        <f>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</f>
+        <v>"TABLE",</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1" t="str">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</f>
         <v>TABLE = 35</v>
       </c>

</xml_diff>

<commit_message>
Additional SQL data type mappings
Was missing System.Byte and System.Int16 in the mappings
</commit_message>
<xml_diff>
--- a/Documentation/SQL Server Data Type Mapping.xlsx
+++ b/Documentation/SQL Server Data Type Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Repos\LightosTomJ\XmlSchemaSQLClassGenerator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E702B6-320E-40BC-82EC-87CA5802D72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B56683E-3961-47D4-8B61-33998A7984AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25500" yWindow="-14250" windowWidth="25820" windowHeight="14020" xr2:uid="{2EBCF0CA-1BBD-4416-BD84-C9160D9783C5}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="19200" windowHeight="10100" xr2:uid="{2EBCF0CA-1BBD-4416-BD84-C9160D9783C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL Server" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>SEARCHABLE</t>
+  </si>
+  <si>
+    <t>System.Int16</t>
+  </si>
+  <si>
+    <t>System.Byte</t>
   </si>
 </sst>
 </file>
@@ -383,9 +389,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -396,6 +399,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -429,13 +435,13 @@
     <tableColumn id="1" xr3:uid="{8071A964-D957-4E5D-9D94-CDD2BCFC720D}" name="Category" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{AD035300-63E1-4FF5-83F2-CE4ABEDB3409}" name="VS.Net Type" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{CB955490-B800-46F0-BD9D-08047E39A4CE}" name="SQL Data type" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{606148DF-C255-4122-95F2-69D75DEFD3BE}" name="SEARCHABLE" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{606148DF-C255-4122-95F2-69D75DEFD3BE}" name="SEARCHABLE" dataDxfId="4">
       <calculatedColumnFormula>IF(ISERROR(FIND("(",Table1[[#This Row],[SQL Data type]])&gt;0),_xlfn.CONCAT(CHAR(34),UPPER(Table1[[#This Row],[SQL Data type]]),CHAR(34),","),_xlfn.CONCAT(CHAR(34),UPPER(MID(Table1[[#This Row],[SQL Data type]],1,FIND("(",Table1[[#This Row],[SQL Data type]])-1)),CHAR(34),","))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E25ED441-D357-49AB-B233-09454A354217}" name="Description" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{13525C3A-CA9B-42DB-B7AB-FF6D3F2D643D}" name="Storage" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{19B6C793-CB81-4243-89C2-337052737FCF}" name="Max size" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{57F8925F-7F1A-4B66-9800-60148EC9CCD9}" name="Enum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{E25ED441-D357-49AB-B233-09454A354217}" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{13525C3A-CA9B-42DB-B7AB-FF6D3F2D643D}" name="Storage" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{19B6C793-CB81-4243-89C2-337052737FCF}" name="Max size" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{57F8925F-7F1A-4B66-9800-60148EC9CCD9}" name="Enum" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(UPPER(Table1[[#This Row],[SQL Data type]]),"(","_"),")","_"),",","-")," = ",ROW()-1,IF((ROW()-1)=ROWS(Table1[]),"",","))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -742,21 +748,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0622978-7C17-40AE-B19F-5EC9DE1E88C1}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
-    <col min="3" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="123.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="3" max="4" width="21.1796875" customWidth="1"/>
+    <col min="5" max="5" width="123.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -782,7 +788,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -808,7 +814,7 @@
         <v>CHAR_N_ = 1,</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -834,7 +840,7 @@
         <v>VARCHAR_N_ = 2,</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -860,7 +866,7 @@
         <v>VARCHAR_MAX_ = 3,</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -886,7 +892,7 @@
         <v>TEXT = 4,</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -912,7 +918,7 @@
         <v>NCHAR = 5,</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -938,7 +944,7 @@
         <v>NVARCHAR = 6,</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -964,7 +970,7 @@
         <v>NVARCHAR_MAX_ = 7,</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -990,7 +996,7 @@
         <v>NTEXT = 8,</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>BINARY_N_ = 9,</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>VARBINARY = 10,</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>VARBINARY_MAX_ = 11,</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>IMAGE = 12,</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1116,11 +1122,13 @@
         <v>BIT = 13,</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1140,11 +1148,13 @@
         <v>TINYINT = 14,</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1164,7 +1174,7 @@
         <v>SMALLINT = 15,</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1200,7 @@
         <v>INT = 16,</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1216,7 +1226,7 @@
         <v>BIGINT = 17,</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1240,7 +1250,7 @@
         <v>DECIMAL_P-S_ = 18,</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1274,7 @@
         <v>NUMERIC_P-S_ = 19,</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>SMALLMONEY = 20,</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +1322,7 @@
         <v>MONEY = 21,</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>FLOAT_N_ = 22,</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>REAL = 23,</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>DATETIME = 24,</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -1408,7 +1418,7 @@
         <v>DATETIME2 = 25,</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
@@ -1432,7 +1442,7 @@
         <v>SMALLDATETIME = 26,</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -1456,7 +1466,7 @@
         <v>DATE = 27,</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
@@ -1480,7 +1490,7 @@
         <v>TIME = 28,</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -1504,7 +1514,7 @@
         <v>DATETIMEOFFSET = 29,</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>TIMESTAMP = 30,</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>SQL_VARIANT = 31,</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
@@ -1572,7 +1582,7 @@
         <v>UNIQUEIDENTIFIER = 32,</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
@@ -1594,7 +1604,7 @@
         <v>XML = 33,</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -1616,7 +1626,7 @@
         <v>CURSOR = 34,</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>

</xml_diff>